<commit_message>
changed gpsManager to register users successfully
</commit_message>
<xml_diff>
--- a/doc/DataDictionary.xlsx
+++ b/doc/DataDictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="118">
   <si>
     <t>user 用户表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,23 +133,171 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activity 活动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>serial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>character varying</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp with time zone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp with time zone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>character varying</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>integer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>create_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act_cate_child/accid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count_like</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a_lat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double precision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a_lon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activity_comment 活动评论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>serial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activity/aid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>yes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>activity 活动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>aid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>serial</t>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp with time zone</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -157,327 +305,187 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>now()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read_by_reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reply_to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read_by_activity_holder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>city 城市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>province</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act_cate_parent/acpid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count_dislike</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_organization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_like_activity 用户喜欢活动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ulaid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activity_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>udaid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_dislike_activity 用户投诉活动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization 组织</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>grade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_valid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act_sub_cate 活动2级标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ascid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act_main_cate 活动1级标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amcid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>character varying</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>end_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>start_time</t>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>character varying</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>timestamp with time zone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>timestamp with time zone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>now()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>character varying</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create_user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user/uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>category</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>act_cate_child/accid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>count_like</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a_lat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>double precision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a_lon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activity_comment 活动评论</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>serial</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activity/aid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user/uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>text</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>timestamp with time zone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>now()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>read_by_reply</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reply_to</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>read_by_activity_holder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>city 城市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>city</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>province</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>parent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>act_cate_parent/acpid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>count_dislike</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is_organization</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_like_activity 用户喜欢活动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ulaid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activity_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>udaid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_dislike_activity 用户投诉活动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>organization 组织</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grade</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is_valid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>level</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>act_sub_cate 活动2级标签</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ascid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>acid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>act_main_cate 活动1级标签</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>amcid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>organization</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>character varying</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>location</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -604,10 +612,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -945,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -960,22 +968,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="21">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="I3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="2:14">
       <c r="B4" s="1" t="s">
@@ -1029,13 +1037,13 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="I5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1055,16 +1063,16 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="I6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -1083,16 +1091,16 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="I7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -1113,13 +1121,13 @@
       </c>
       <c r="G8" s="3"/>
       <c r="I8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1141,18 +1149,18 @@
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:14">
@@ -1169,7 +1177,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="I10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>16</v>
@@ -1197,16 +1205,16 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -1216,16 +1224,16 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>16</v>
@@ -1234,7 +1242,7 @@
         <v>9</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3" t="b">
@@ -1246,10 +1254,10 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1257,13 +1265,13 @@
     </row>
     <row r="14" spans="2:14">
       <c r="B14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1272,21 +1280,21 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="21">
-      <c r="I15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+      <c r="I15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
     </row>
     <row r="16" spans="2:14">
       <c r="I16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>3</v>
@@ -1302,16 +1310,16 @@
       </c>
     </row>
     <row r="17" spans="2:14" ht="21">
-      <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="B17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
       <c r="I17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>8</v>
@@ -1343,10 +1351,10 @@
         <v>6</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>9</v>
@@ -1357,22 +1365,22 @@
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>9</v>
@@ -1384,23 +1392,23 @@
       </c>
     </row>
     <row r="20" spans="2:14">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>9</v>
@@ -1411,10 +1419,10 @@
     </row>
     <row r="21" spans="2:14">
       <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
@@ -1425,13 +1433,13 @@
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1439,10 +1447,10 @@
     </row>
     <row r="23" spans="2:14" ht="21">
       <c r="B23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>9</v>
@@ -1450,29 +1458,29 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="I23" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
+      <c r="I23" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>1</v>
@@ -1495,19 +1503,19 @@
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="I25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>8</v>
@@ -1521,24 +1529,24 @@
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="I26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>9</v>
@@ -1549,26 +1557,26 @@
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>9</v>
@@ -1581,10 +1589,10 @@
     </row>
     <row r="29" spans="2:14" ht="21">
       <c r="B29" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>9</v>
@@ -1594,24 +1602,24 @@
       <c r="G29" s="3">
         <v>0</v>
       </c>
-      <c r="I29" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
+      <c r="I29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1639,10 +1647,10 @@
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>17</v>
@@ -1651,7 +1659,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="I31" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>8</v>
@@ -1665,10 +1673,10 @@
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>17</v>
@@ -1677,10 +1685,10 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>9</v>
@@ -1691,29 +1699,29 @@
     </row>
     <row r="33" spans="2:14">
       <c r="I33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
     <row r="35" spans="2:14" ht="21">
-      <c r="B35" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="B35" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36" spans="2:14" ht="21">
       <c r="B36" s="1" t="s">
@@ -1734,18 +1742,18 @@
       <c r="G36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
+      <c r="I36" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
     </row>
     <row r="37" spans="2:14">
       <c r="B37" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>8</v>
@@ -1777,21 +1785,21 @@
     </row>
     <row r="38" spans="2:14">
       <c r="B38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="I38" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>8</v>
@@ -1800,34 +1808,34 @@
         <v>9</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="2:14">
       <c r="B39" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="I39" s="6" t="s">
+      <c r="I39" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J39" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="K39" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -1835,10 +1843,10 @@
     </row>
     <row r="40" spans="2:14">
       <c r="I40" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>9</v>
@@ -1849,32 +1857,32 @@
     </row>
     <row r="41" spans="2:14">
       <c r="I41" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
     </row>
     <row r="42" spans="2:14" ht="21">
-      <c r="B42" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="B42" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
       <c r="I42" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J42" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>9</v>
@@ -1905,7 +1913,7 @@
     </row>
     <row r="44" spans="2:14">
       <c r="B44" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>8</v>
@@ -1919,32 +1927,32 @@
     </row>
     <row r="45" spans="2:14">
       <c r="B45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="2:14">
       <c r="B46" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>

</xml_diff>

<commit_message>
Changed the name of dataEncrpytionStorage and added upper level api for sqlite database
</commit_message>
<xml_diff>
--- a/doc/DataDictionary.xlsx
+++ b/doc/DataDictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="121">
   <si>
     <t>user 用户表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -257,11 +257,239 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>activity/aid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp with time zone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read_by_reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read_by_activity_holder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>city 城市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>province</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act_cate_parent/acpid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count_dislike</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_organization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_like_activity 用户喜欢活动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ulaid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activity_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>udaid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_dislike_activity 用户投诉活动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization 组织</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_valid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act_sub_cate 活动2级标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ascid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act_main_cate 活动1级标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amcid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>character varying</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>character varying</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp with time zone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>activity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>activity/aid</t>
+    <t>reply_to</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -269,235 +497,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>user/uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>text</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>timestamp with time zone</t>
+    <t>aid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>now()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>read_by_reply</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>read_by_activity_holder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>city 城市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>city</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>province</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>parent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>act_cate_parent/acpid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>count_dislike</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is_organization</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_like_activity 用户喜欢活动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ulaid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activity_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>udaid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_dislike_activity 用户投诉活动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>organization 组织</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grade</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is_valid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>level</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>act_sub_cate 活动2级标签</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ascid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>acid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>act_main_cate 活动1级标签</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>amcid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>organization</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>character varying</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>character varying</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>timestamp with time zone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>city</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reply_to</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -961,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1045,7 +1049,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="I5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>57</v>
@@ -1071,7 +1075,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="I6" s="4" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>46</v>
@@ -1080,7 +1084,7 @@
         <v>9</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -1101,7 +1105,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>46</v>
@@ -1110,7 +1114,7 @@
         <v>9</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -1131,13 +1135,13 @@
         <v>1</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1157,18 +1161,18 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="I9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:14">
@@ -1187,24 +1191,26 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="I10" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="N10" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>26</v>
@@ -1213,7 +1219,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>46</v>
@@ -1222,7 +1228,7 @@
         <v>15</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -1232,16 +1238,16 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>14</v>
@@ -1250,7 +1256,7 @@
         <v>9</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3" t="b">
@@ -1259,13 +1265,13 @@
     </row>
     <row r="13" spans="2:14">
       <c r="B13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1275,7 +1281,7 @@
     </row>
     <row r="15" spans="2:14" ht="21">
       <c r="I15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1296,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>3</v>
@@ -1331,7 +1337,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>8</v>
@@ -1357,7 +1363,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>32</v>
@@ -1371,19 +1377,19 @@
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>46</v>
@@ -1411,7 +1417,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>32</v>
@@ -1431,7 +1437,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1467,7 +1473,7 @@
         <v>39</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -1477,13 +1483,13 @@
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1523,7 +1529,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="I25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>8</v>
@@ -1581,7 +1587,7 @@
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>46</v>
@@ -1611,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -1665,7 +1671,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="I31" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>8</v>
@@ -1679,13 +1685,13 @@
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>45</v>
@@ -1702,23 +1708,23 @@
     </row>
     <row r="33" spans="2:14">
       <c r="I33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J33" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" ht="21">
       <c r="B34" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1748,7 +1754,7 @@
     </row>
     <row r="36" spans="2:14" ht="21">
       <c r="B36" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>8</v>
@@ -1760,7 +1766,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="I36" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
@@ -1770,7 +1776,7 @@
     </row>
     <row r="37" spans="2:14">
       <c r="B37" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>46</v>
@@ -1779,7 +1785,7 @@
         <v>9</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -1804,7 +1810,7 @@
     </row>
     <row r="38" spans="2:14">
       <c r="B38" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>46</v>
@@ -1813,12 +1819,12 @@
         <v>9</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="I38" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>8</v>
@@ -1827,20 +1833,20 @@
         <v>9</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="2:14">
       <c r="I39" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J39" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="K39" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -1848,7 +1854,7 @@
     </row>
     <row r="40" spans="2:14">
       <c r="I40" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>32</v>
@@ -1862,7 +1868,7 @@
     </row>
     <row r="41" spans="2:14" ht="21">
       <c r="B41" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -1870,13 +1876,13 @@
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="I41" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>46</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -1902,10 +1908,10 @@
         <v>6</v>
       </c>
       <c r="I42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J42" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>9</v>
@@ -1916,7 +1922,7 @@
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>8</v>
@@ -1930,7 +1936,7 @@
     </row>
     <row r="44" spans="2:14">
       <c r="B44" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>46</v>
@@ -1939,14 +1945,14 @@
         <v>9</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="2:14">
       <c r="B45" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>46</v>
@@ -1955,7 +1961,7 @@
         <v>9</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>

</xml_diff>